<commit_message>
made data fiels final in store, staff and customer classes and updated README file
</commit_message>
<xml_diff>
--- a/src/main/resources/shopwell-inventory.xlsx
+++ b/src/main/resources/shopwell-inventory.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Samsung TV</t>
+  </si>
+  <si>
+    <t>iPhone 14 Pro</t>
   </si>
 </sst>
 </file>
@@ -508,6 +511,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>